<commit_message>
Updated charts to include TX2 times
</commit_message>
<xml_diff>
--- a/logs/Platform Timings.xlsx
+++ b/logs/Platform Timings.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisemcellhiney/Documents/School/Research/picar/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,15 +30,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>Raspberry Pi 3</t>
   </si>
   <si>
     <t>Intel UP Board</t>
-  </si>
-  <si>
-    <t>NVIDIA Tegra TX2</t>
   </si>
   <si>
     <t>2 model</t>
@@ -51,6 +54,24 @@
   </si>
   <si>
     <t>4 core</t>
+  </si>
+  <si>
+    <t>NVIDIA Tegra TX2 CPU only</t>
+  </si>
+  <si>
+    <t>NVIDIA Tegra TX2 GPU</t>
+  </si>
+  <si>
+    <t>1 benchmark</t>
+  </si>
+  <si>
+    <t>0 benchmarks</t>
+  </si>
+  <si>
+    <t>2 benchmarks</t>
+  </si>
+  <si>
+    <t>3 benchmarks</t>
   </si>
 </sst>
 </file>
@@ -234,10 +255,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>58.014496586999996</c:v>
+                  <c:v>58.014496587</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.359130105700004</c:v>
+                  <c:v>78.3591301057</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,10 +370,236 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>23.808301090299999</c:v>
+                  <c:v>23.8083010903</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.353692072400001</c:v>
+                  <c:v>39.3536920724</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NVIDIA Tegra TX2 CPU only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$11:$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2 model</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4 model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NVIDIA Tegra TX2 GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$11:$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2 model</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4 model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -369,11 +616,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1204743424"/>
-        <c:axId val="1204745600"/>
+        <c:axId val="-10604560"/>
+        <c:axId val="-10595728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1204743424"/>
+        <c:axId val="-10604560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -477,7 +724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1204745600"/>
+        <c:crossAx val="-10595728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -485,7 +732,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1204745600"/>
+        <c:axId val="-10595728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +839,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1204743424"/>
+        <c:crossAx val="-10604560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -807,13 +1054,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>62.463862069500003</c:v>
+                  <c:v>62.4638620695</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.652717217599999</c:v>
+                  <c:v>50.6527172176</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.530173879899998</c:v>
+                  <c:v>48.5301738799</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>43.2479538013</c:v>
@@ -934,16 +1181,266 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>30.977631091399999</c:v>
+                  <c:v>30.9776310914</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.045440954099998</c:v>
+                  <c:v>21.0454409541</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.483242157399999</c:v>
+                  <c:v>19.4832421574</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.082677928300001</c:v>
+                  <c:v>17.0826779283</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NVIDIA Tegra TX2 CPU only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1 core</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 core</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 core</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4 core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NVIDIA Tegra TX2 GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1 core</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 core</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 core</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4 core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -960,11 +1457,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1204747232"/>
-        <c:axId val="1204749408"/>
+        <c:axId val="-10439120"/>
+        <c:axId val="-10430480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1204747232"/>
+        <c:axId val="-10439120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1063,7 +1560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1204749408"/>
+        <c:crossAx val="-10430480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1071,7 +1568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1204749408"/>
+        <c:axId val="-10430480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,7 +1675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1204747232"/>
+        <c:crossAx val="-10439120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1390,13 +1887,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>623.49172937699996</c:v>
+                  <c:v>623.491729377</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>391.65209737599997</c:v>
+                  <c:v>391.652097376</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.916486734700001</c:v>
+                  <c:v>98.9164867347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1511,14 +2008,232 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>70.471428260300002</c:v>
+                  <c:v>70.4714282603</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>35.6551400265</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.796047659599999</c:v>
-                </c:pt>
+                  <c:v>29.7960476596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NVIDIA Tegra TX2 CPU only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$20:$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1 core</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 core</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NVIDIA Tegra TX2 GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$20:$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1 core</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 core</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1534,11 +2249,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1204749952"/>
-        <c:axId val="1204753216"/>
+        <c:axId val="-10354096"/>
+        <c:axId val="-10345488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1204749952"/>
+        <c:axId val="-10354096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +2352,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1204753216"/>
+        <c:crossAx val="-10345488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1645,7 +2360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1204753216"/>
+        <c:axId val="-10345488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1752,7 +2467,596 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1204749952"/>
+        <c:crossAx val="-10354096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Raspberry Pi 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$30:$E$30</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0 benchmarks</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 benchmark</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 benchmarks</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 benchmarks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$31:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>62.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel UP Board</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$30:$E$30</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0 benchmarks</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 benchmark</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 benchmarks</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 benchmarks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$32:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>30.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NVIDIA Tegra TX2 CPU only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$30:$E$30</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0 benchmarks</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 benchmark</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 benchmarks</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 benchmarks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$33:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NVIDIA Tegra TX2 GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$30:$E$30</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0 benchmarks</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 benchmark</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 benchmarks</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 benchmarks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$34:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="42086816"/>
+        <c:axId val="60251056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="42086816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of benchmarks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60251056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="60251056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Inferencing Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="42086816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1953,6 +3257,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2960,6 +4304,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3549,6 +5396,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3820,38 +5697,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3868,7 +5746,7 @@
         <v>43.2479538013</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3885,20 +5763,49 @@
         <v>17.082677928300001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>20.65</v>
+      </c>
+      <c r="C4">
+        <v>14.52</v>
+      </c>
+      <c r="D4">
+        <v>13.55</v>
+      </c>
+      <c r="E4">
+        <v>12.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>6.9</v>
+      </c>
+      <c r="C5">
+        <v>5.83</v>
+      </c>
+      <c r="D5">
+        <v>5.74</v>
+      </c>
+      <c r="E5">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>2</v>
       </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -3909,7 +5816,7 @@
         <v>78.359130105700004</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -3920,23 +5827,40 @@
         <v>39.353692072400001</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>24.48</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>7.33</v>
+      </c>
+      <c r="C15">
+        <v>8.81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -3950,7 +5874,7 @@
         <v>98.916486734700001</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -3964,9 +5888,89 @@
         <v>29.796047659599999</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>62.46</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1">
+        <v>30.98</v>
+      </c>
+      <c r="C32" s="1">
+        <v>41.87</v>
+      </c>
+      <c r="D32" s="1">
+        <v>60.6</v>
+      </c>
+      <c r="E32" s="1">
+        <v>70.47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>20.65</v>
+      </c>
+      <c r="C33">
+        <v>26.1</v>
+      </c>
+      <c r="D33">
+        <v>36.630000000000003</v>
+      </c>
+      <c r="E33">
+        <v>44.95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>6.9</v>
+      </c>
+      <c r="C34">
+        <v>10.71</v>
+      </c>
+      <c r="D34">
+        <v>12.84</v>
+      </c>
+      <c r="E34">
+        <v>16.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added labels to chart
</commit_message>
<xml_diff>
--- a/logs/Platform Timings.xlsx
+++ b/logs/Platform Timings.xlsx
@@ -2596,6 +2596,65 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$30:$E$30</c:f>
@@ -2655,6 +2714,65 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$30:$E$30</c:f>
@@ -2721,6 +2839,65 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$30:$E$30</c:f>
@@ -2787,6 +2964,65 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$30:$E$30</c:f>
@@ -2830,8 +3066,9 @@
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -5699,7 +5936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added Pi3 times to benchmark chart
</commit_message>
<xml_diff>
--- a/logs/Platform Timings.xlsx
+++ b/logs/Platform Timings.xlsx
@@ -2683,6 +2683,15 @@
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>62.46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>104.16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>298.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>588.3099999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5936,8 +5945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6156,8 +6165,15 @@
       <c r="B31" s="1">
         <v>62.46</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="C31" s="1">
+        <v>104.16</v>
+      </c>
+      <c r="D31" s="1">
+        <v>298</v>
+      </c>
+      <c r="E31" s="1">
+        <v>588.30999999999995</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">

</xml_diff>

<commit_message>
Update values/figure for model comparison
Added values for 1Nx1C and 1Nx2C. Also update the values for the UP
Board since they were from older tests.
</commit_message>
<xml_diff>
--- a/logs/Platform Timings.xlsx
+++ b/logs/Platform Timings.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisemcellhiney/Documents/School/Research/picar/logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbech\Documents\picar\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="28725" windowHeight="17535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>Raspberry Pi 3</t>
   </si>
@@ -73,11 +73,14 @@
   <si>
     <t>3 benchmarks</t>
   </si>
+  <si>
+    <t>dual core</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,7 +131,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -215,7 +218,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -236,33 +238,32 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$11:$C$11</c:f>
+              <c:f>Sheet1!$D$11:$D$11</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 model</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4 model</c:v>
+                  <c:v>dual core</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$C$12</c:f>
+              <c:f>Sheet1!$D$12:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>58.014496587</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>78.3591301057</c:v>
+                  <c:v>50.652717217599999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6667-47AD-8319-7E636E73DB65}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -330,7 +331,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -351,33 +351,32 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$11:$C$11</c:f>
+              <c:f>Sheet1!$D$11:$D$11</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 model</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4 model</c:v>
+                  <c:v>dual core</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$C$13</c:f>
+              <c:f>Sheet1!$D$13:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>23.8083010903</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>39.3536920724</c:v>
+                  <c:v>22.2140382258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6667-47AD-8319-7E636E73DB65}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -443,7 +442,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -464,33 +462,32 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$11:$C$11</c:f>
+              <c:f>Sheet1!$D$11:$D$11</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 model</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4 model</c:v>
+                  <c:v>dual core</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$C$14</c:f>
+              <c:f>Sheet1!$D$14:$D$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24.48</c:v>
+                  <c:v>14.521577048699999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6667-47AD-8319-7E636E73DB65}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -556,7 +553,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -577,33 +573,32 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$11:$C$11</c:f>
+              <c:f>Sheet1!$D$11:$D$11</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 model</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4 model</c:v>
+                  <c:v>dual core</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$C$15</c:f>
+              <c:f>Sheet1!$D$15:$D$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7.33</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.81</c:v>
+                  <c:v>5.8322707868699997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6667-47AD-8319-7E636E73DB65}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
@@ -657,7 +652,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -778,7 +772,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -853,7 +846,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -921,7 +913,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1008,7 +1000,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1054,13 +1045,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>62.4638620695</c:v>
+                  <c:v>62.463862069500003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.6527172176</c:v>
+                  <c:v>50.652717217599999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.5301738799</c:v>
+                  <c:v>48.530173879899998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>43.2479538013</c:v>
@@ -1068,6 +1059,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A42C-4E9B-AB7B-20225891A446}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1135,7 +1131,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1181,20 +1176,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>30.9776310914</c:v>
+                  <c:v>30.977631091399999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.0454409541</c:v>
+                  <c:v>21.045440954099998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.4832421574</c:v>
+                  <c:v>19.483242157399999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.0826779283</c:v>
+                  <c:v>17.082677928300001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A42C-4E9B-AB7B-20225891A446}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1260,7 +1260,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1320,6 +1319,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A42C-4E9B-AB7B-20225891A446}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1385,7 +1389,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1445,6 +1448,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A42C-4E9B-AB7B-20225891A446}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
@@ -1493,7 +1501,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1614,7 +1621,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1689,7 +1695,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1757,7 +1762,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1844,7 +1849,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1887,17 +1891,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>623.491729377</c:v>
+                  <c:v>623.49172937699996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>391.652097376</c:v>
+                  <c:v>391.65209737599997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.9164867347</c:v>
+                  <c:v>98.916486734700001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B37D-4C53-9EC8-6B6C5474382A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1965,7 +1974,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2008,17 +2016,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>70.4714282603</c:v>
+                  <c:v>70.471428260300002</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>35.6551400265</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.7960476596</c:v>
+                  <c:v>29.796047659599999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B37D-4C53-9EC8-6B6C5474382A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2128,6 +2141,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B37D-4C53-9EC8-6B6C5474382A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2237,6 +2255,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B37D-4C53-9EC8-6B6C5474382A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
@@ -2285,7 +2308,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2406,7 +2428,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2481,7 +2502,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2549,7 +2569,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2636,7 +2656,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2688,14 +2707,19 @@
                   <c:v>104.16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>298.0</c:v>
+                  <c:v>298</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>588.3099999999999</c:v>
+                  <c:v>588.30999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FB33-4E69-B19E-143D39EE4FAB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2763,7 +2787,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2823,6 +2846,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FB33-4E69-B19E-143D39EE4FAB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2888,7 +2916,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2940,7 +2967,7 @@
                   <c:v>26.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.63</c:v>
+                  <c:v>36.630000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>44.95</c:v>
@@ -2948,6 +2975,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FB33-4E69-B19E-143D39EE4FAB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -3013,7 +3045,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3073,6 +3104,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FB33-4E69-B19E-143D39EE4FAB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
@@ -3121,7 +3157,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3242,7 +3277,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3272,6 +3306,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3316,7 +3351,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5945,23 +5979,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -5975,7 +6010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5992,7 +6027,7 @@
         <v>43.2479538013</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6009,7 +6044,7 @@
         <v>17.082677928300001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -6026,7 +6061,7 @@
         <v>12.06</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -6043,59 +6078,89 @@
         <v>5.67</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1">
-        <v>58.014496586999996</v>
+        <v>62.463862069500003</v>
       </c>
       <c r="C12" s="1">
         <v>78.359130105700004</v>
       </c>
+      <c r="D12" s="1">
+        <v>50.652717217599999</v>
+      </c>
+      <c r="E12" s="1">
+        <v>58.014496586999996</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>23.808301090299999</v>
+        <v>31.1265648177</v>
       </c>
       <c r="C13" s="1">
-        <v>39.353692072400001</v>
+        <v>44.6246122668</v>
+      </c>
+      <c r="D13" s="1">
+        <v>22.2140382258</v>
+      </c>
+      <c r="E13" s="1">
+        <v>26.8852931797</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14">
-        <v>16</v>
+      <c r="B14" s="1">
+        <v>20.654251844200001</v>
       </c>
       <c r="C14">
         <v>24.48</v>
       </c>
+      <c r="D14" s="1">
+        <v>14.521577048699999</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15">
-        <v>7.33</v>
+      <c r="B15" s="1">
+        <v>6.8984385393799998</v>
       </c>
       <c r="C15">
         <v>8.81</v>
       </c>
+      <c r="D15" s="1">
+        <v>5.8322707868699997</v>
+      </c>
+      <c r="E15">
+        <v>7.33</v>
+      </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -6106,7 +6171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -6120,7 +6185,7 @@
         <v>98.916486734700001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -6134,17 +6199,17 @@
         <v>29.796047659599999</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>11</v>
       </c>
@@ -6158,7 +6223,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -6175,7 +6240,7 @@
         <v>588.30999999999995</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -6192,7 +6257,7 @@
         <v>70.47</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -6209,7 +6274,7 @@
         <v>44.95</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>

</xml_diff>